<commit_message>
read directory and templet done
</commit_message>
<xml_diff>
--- a/directory.xlsx
+++ b/directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Jones Lang LaSalle, JLL\353 Sacramento, SF\Yodeck.com\custom apps\directory\Customizable-Directory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6C80F7-4E39-4E6F-815F-BBA14ACED565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9A33E2-2108-447C-B0DC-2BC72B35F793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,52 +360,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:C8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>200</v>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2200</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="B6">
         <v>360</v>
       </c>
     </row>

</xml_diff>